<commit_message>
Json Scraped Full Data, Criteria Validation update
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/IngredientsAndComorbidities-ScrapperHackathon.xlsx
+++ b/src/test/resources/testdata/IngredientsAndComorbidities-ScrapperHackathon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Febi\NumpyNinja\Hackathon\RecipeScrapingHackathon_July24\RecipeScraping\Team11_ScrapeTechies_ScrapingHackthonJuly24\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF31F25-E260-4510-AB88-7DC69987FC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E3BFA6-063C-44B3-BD1A-FA44A7AE2A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1198,13 +1198,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1218,6 +1211,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="&quot;Helvetica Neue&quot;"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1481,13 +1481,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1498,6 +1497,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1734,22 +1734,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="26" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="26" t="s">
+      <c r="D1" s="26"/>
+      <c r="E1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="26" t="s">
+      <c r="F1" s="26"/>
+      <c r="G1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="27"/>
+      <c r="H1" s="26"/>
       <c r="I1" s="1"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -30054,8 +30054,8 @@
   </sheetPr>
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -30071,13 +30071,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="28" customHeight="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
       <c r="A2" s="17" t="s">
@@ -30198,22 +30198,22 @@
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
     </row>
-    <row r="10" spans="1:8" ht="13">
+    <row r="10" spans="1:8" ht="12.5">
       <c r="A10" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
     </row>
-    <row r="11" spans="1:8" ht="13">
+    <row r="11" spans="1:8" ht="12.5">
       <c r="A11" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="29" t="s">
         <v>159</v>
       </c>
       <c r="C11" s="18"/>
@@ -30571,7 +30571,7 @@
       <c r="B43" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="C43" s="22"/>
+      <c r="C43" s="21"/>
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
     </row>
@@ -30604,7 +30604,7 @@
       <c r="B46" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="C46" s="22"/>
+      <c r="C46" s="21"/>
       <c r="D46" s="18"/>
       <c r="E46" s="18"/>
     </row>
@@ -31092,12 +31092,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="35.5" customHeight="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="27" t="s">
         <v>302</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1">
       <c r="A2" s="17" t="s">
@@ -31120,10 +31120,10 @@
       <c r="B3" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>305</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>306</v>
       </c>
     </row>
@@ -31135,7 +31135,7 @@
         <v>170</v>
       </c>
       <c r="C4" s="18"/>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="23" t="s">
         <v>308</v>
       </c>
     </row>
@@ -31147,7 +31147,7 @@
         <v>310</v>
       </c>
       <c r="C5" s="18"/>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>311</v>
       </c>
     </row>
@@ -31159,7 +31159,7 @@
         <v>168</v>
       </c>
       <c r="C6" s="18"/>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>313</v>
       </c>
     </row>
@@ -31171,7 +31171,7 @@
         <v>314</v>
       </c>
       <c r="C7" s="18"/>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="23" t="s">
         <v>315</v>
       </c>
     </row>
@@ -31183,7 +31183,7 @@
         <v>61</v>
       </c>
       <c r="C8" s="18"/>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>316</v>
       </c>
     </row>
@@ -31195,7 +31195,7 @@
         <v>318</v>
       </c>
       <c r="C9" s="18"/>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>319</v>
       </c>
     </row>
@@ -31947,67 +31947,67 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="15" customHeight="1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15" customHeight="1">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15" customHeight="1">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15" customHeight="1">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15" customHeight="1">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="24" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15" customHeight="1">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15" customHeight="1">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="24" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15" customHeight="1">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="24" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15" customHeight="1">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="24" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15" customHeight="1">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15" customHeight="1">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15" customHeight="1">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="24" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15" customHeight="1">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>369</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Structure changes and LCHF Allergy update
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/IngredientsAndComorbidities-ScrapperHackathon.xlsx
+++ b/src/test/resources/testdata/IngredientsAndComorbidities-ScrapperHackathon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Febi\NumpyNinja\Hackathon\RecipeScrapingHackathon_July24\RecipeScraping\Team11_ScrapeTechies_ScrapingHackthonJuly24\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E3BFA6-063C-44B3-BD1A-FA44A7AE2A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49D9FCA-AB4C-4EF7-92CA-C3044E74BD19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="371">
   <si>
     <t>Diabetes</t>
   </si>
@@ -444,9 +444,6 @@
     <t>ghee</t>
   </si>
   <si>
-    <t>microwave meals or ready meals</t>
-  </si>
-  <si>
     <t>Coffee or tea without sugar</t>
   </si>
   <si>
@@ -678,15 +675,9 @@
     <t>tangerine</t>
   </si>
   <si>
-    <t>all berry varieties</t>
-  </si>
-  <si>
     <t>pastry</t>
   </si>
   <si>
-    <t>all melon varieties</t>
-  </si>
-  <si>
     <t>cakes</t>
   </si>
   <si>
@@ -885,9 +876,6 @@
     <t>stevia</t>
   </si>
   <si>
-    <t>all forms of chana</t>
-  </si>
-  <si>
     <t>barley malt</t>
   </si>
   <si>
@@ -1138,6 +1126,21 @@
   </si>
   <si>
     <t>Seafood</t>
+  </si>
+  <si>
+    <t>Peanut</t>
+  </si>
+  <si>
+    <t>melon</t>
+  </si>
+  <si>
+    <t>berry</t>
+  </si>
+  <si>
+    <t>chana</t>
+  </si>
+  <si>
+    <t>microwave</t>
   </si>
 </sst>
 </file>
@@ -1214,7 +1217,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1489,6 +1491,7 @@
     <xf numFmtId="49" fontId="11" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1497,7 +1500,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1734,22 +1736,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="25" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="25" t="s">
+      <c r="D1" s="27"/>
+      <c r="E1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="25" t="s">
+      <c r="F1" s="27"/>
+      <c r="G1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="26"/>
+      <c r="H1" s="27"/>
       <c r="I1" s="1"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -30055,7 +30057,7 @@
   <dimension ref="A1:J90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -30070,14 +30072,14 @@
     <col min="10" max="10" width="18.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28" customHeight="1">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:8" ht="15" customHeight="1">
+      <c r="A1" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1">
       <c r="A2" s="17" t="s">
@@ -30124,75 +30126,75 @@
         <v>137</v>
       </c>
       <c r="D4" s="19" t="s">
+        <v>370</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>138</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1">
       <c r="A5" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="C5" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="D5" s="18" t="s">
         <v>142</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>143</v>
       </c>
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
       <c r="A6" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="C6" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="D6" s="18" t="s">
         <v>146</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>147</v>
       </c>
       <c r="E6" s="18"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1">
       <c r="A7" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="C7" s="18" t="s">
         <v>149</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>150</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
       <c r="A8" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>151</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>152</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
       <c r="H8" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1">
       <c r="A9" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>154</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>155</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
@@ -30200,10 +30202,10 @@
     </row>
     <row r="10" spans="1:8" ht="12.5">
       <c r="A10" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="B10" s="25" t="s">
         <v>156</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>157</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="18"/>
@@ -30211,10 +30213,10 @@
     </row>
     <row r="11" spans="1:8" ht="12.5">
       <c r="A11" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="B11" s="25" t="s">
         <v>158</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>159</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
@@ -30222,10 +30224,10 @@
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1">
       <c r="A12" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>160</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>161</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
@@ -30233,10 +30235,10 @@
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1">
       <c r="A13" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="B13" s="18" t="s">
         <v>162</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>163</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -30244,10 +30246,10 @@
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1">
       <c r="A14" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>164</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>165</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
@@ -30255,10 +30257,10 @@
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1">
       <c r="A15" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>166</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>167</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
@@ -30266,10 +30268,10 @@
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1">
       <c r="A16" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>168</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>169</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
@@ -30277,10 +30279,10 @@
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1">
       <c r="A17" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="B17" s="18" t="s">
         <v>170</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>171</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
@@ -30288,24 +30290,24 @@
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1">
       <c r="A18" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="B18" s="18" t="s">
         <v>172</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>173</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
       <c r="J18" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1">
       <c r="A19" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>175</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>176</v>
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
@@ -30313,10 +30315,10 @@
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1">
       <c r="A20" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="B20" s="18" t="s">
         <v>177</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>178</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
@@ -30324,10 +30326,10 @@
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1">
       <c r="A21" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="B21" s="18" t="s">
         <v>179</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>180</v>
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
@@ -30335,10 +30337,10 @@
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1">
       <c r="A22" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="B22" s="18" t="s">
         <v>181</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>182</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
@@ -30346,10 +30348,10 @@
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1">
       <c r="A23" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="B23" s="18" t="s">
         <v>183</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>184</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
@@ -30357,10 +30359,10 @@
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1">
       <c r="A24" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
@@ -30368,10 +30370,10 @@
     </row>
     <row r="25" spans="1:10" ht="15" customHeight="1">
       <c r="A25" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="B25" s="18" t="s">
         <v>186</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>187</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
@@ -30379,10 +30381,10 @@
     </row>
     <row r="26" spans="1:10" ht="12.5">
       <c r="A26" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="B26" s="18" t="s">
         <v>188</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>189</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
@@ -30390,10 +30392,10 @@
     </row>
     <row r="27" spans="1:10" ht="12.5">
       <c r="A27" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="B27" s="18" t="s">
         <v>190</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>191</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
@@ -30401,10 +30403,10 @@
     </row>
     <row r="28" spans="1:10" ht="12.5">
       <c r="A28" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="B28" s="18" t="s">
         <v>192</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>193</v>
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
@@ -30412,10 +30414,10 @@
     </row>
     <row r="29" spans="1:10" ht="12.5">
       <c r="A29" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="B29" s="18" t="s">
         <v>194</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>195</v>
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
@@ -30423,10 +30425,10 @@
     </row>
     <row r="30" spans="1:10" ht="12.5">
       <c r="A30" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="B30" s="18" t="s">
         <v>196</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>197</v>
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="18"/>
@@ -30434,10 +30436,10 @@
     </row>
     <row r="31" spans="1:10" ht="12.5">
       <c r="A31" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="B31" s="18" t="s">
         <v>198</v>
-      </c>
-      <c r="B31" s="18" t="s">
-        <v>199</v>
       </c>
       <c r="C31" s="18"/>
       <c r="D31" s="18"/>
@@ -30445,10 +30447,10 @@
     </row>
     <row r="32" spans="1:10" ht="12.5">
       <c r="A32" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="B32" s="18" t="s">
         <v>200</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>201</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="18"/>
@@ -30456,10 +30458,10 @@
     </row>
     <row r="33" spans="1:5" ht="12.5">
       <c r="A33" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B33" s="18" t="s">
         <v>202</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>203</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
@@ -30467,10 +30469,10 @@
     </row>
     <row r="34" spans="1:5" ht="12.5">
       <c r="A34" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="B34" s="18" t="s">
         <v>204</v>
-      </c>
-      <c r="B34" s="18" t="s">
-        <v>205</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
@@ -30478,10 +30480,10 @@
     </row>
     <row r="35" spans="1:5" ht="12.5">
       <c r="A35" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="B35" s="18" t="s">
         <v>206</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>207</v>
       </c>
       <c r="C35" s="19"/>
       <c r="D35" s="18"/>
@@ -30489,10 +30491,10 @@
     </row>
     <row r="36" spans="1:5" ht="12.5">
       <c r="A36" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="B36" s="18" t="s">
         <v>208</v>
-      </c>
-      <c r="B36" s="18" t="s">
-        <v>209</v>
       </c>
       <c r="C36" s="19"/>
       <c r="D36" s="18"/>
@@ -30500,10 +30502,10 @@
     </row>
     <row r="37" spans="1:5" ht="12.5">
       <c r="A37" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="B37" s="18" t="s">
         <v>210</v>
-      </c>
-      <c r="B37" s="18" t="s">
-        <v>211</v>
       </c>
       <c r="C37" s="19"/>
       <c r="D37" s="18"/>
@@ -30511,10 +30513,10 @@
     </row>
     <row r="38" spans="1:5" ht="12.5">
       <c r="A38" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="B38" s="18" t="s">
         <v>212</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>213</v>
       </c>
       <c r="C38" s="19"/>
       <c r="D38" s="18"/>
@@ -30522,10 +30524,10 @@
     </row>
     <row r="39" spans="1:5" ht="12.5">
       <c r="A39" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="B39" s="18" t="s">
         <v>214</v>
-      </c>
-      <c r="B39" s="18" t="s">
-        <v>215</v>
       </c>
       <c r="C39" s="19"/>
       <c r="D39" s="18"/>
@@ -30536,7 +30538,7 @@
         <v>21</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>216</v>
+        <v>368</v>
       </c>
       <c r="C40" s="19"/>
       <c r="D40" s="18"/>
@@ -30544,10 +30546,10 @@
     </row>
     <row r="41" spans="1:5" ht="12.5">
       <c r="A41" s="18" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>218</v>
+        <v>367</v>
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
@@ -30555,10 +30557,10 @@
     </row>
     <row r="42" spans="1:5" ht="12.5">
       <c r="A42" s="18" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
@@ -30566,10 +30568,10 @@
     </row>
     <row r="43" spans="1:5" ht="12.5">
       <c r="A43" s="18" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C43" s="21"/>
       <c r="D43" s="18"/>
@@ -30577,10 +30579,10 @@
     </row>
     <row r="44" spans="1:5" ht="12.5">
       <c r="A44" s="18" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C44" s="18"/>
       <c r="D44" s="18"/>
@@ -30588,10 +30590,10 @@
     </row>
     <row r="45" spans="1:5" ht="12.5">
       <c r="A45" s="18" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
@@ -30599,10 +30601,10 @@
     </row>
     <row r="46" spans="1:5" ht="12.5">
       <c r="A46" s="18" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C46" s="21"/>
       <c r="D46" s="18"/>
@@ -30610,10 +30612,10 @@
     </row>
     <row r="47" spans="1:5" ht="12.5">
       <c r="A47" s="18" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C47" s="18"/>
       <c r="D47" s="18"/>
@@ -30621,10 +30623,10 @@
     </row>
     <row r="48" spans="1:5" ht="12.5">
       <c r="A48" s="18" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C48" s="18"/>
       <c r="D48" s="18"/>
@@ -30632,10 +30634,10 @@
     </row>
     <row r="49" spans="1:5" ht="12.5">
       <c r="A49" s="18" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C49" s="18"/>
       <c r="D49" s="18"/>
@@ -30643,10 +30645,10 @@
     </row>
     <row r="50" spans="1:5" ht="12.5">
       <c r="A50" s="18" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C50" s="18"/>
       <c r="D50" s="18"/>
@@ -30654,10 +30656,10 @@
     </row>
     <row r="51" spans="1:5" ht="12.5">
       <c r="A51" s="18" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C51" s="18"/>
       <c r="D51" s="18"/>
@@ -30665,10 +30667,10 @@
     </row>
     <row r="52" spans="1:5" ht="12.5">
       <c r="A52" s="18" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C52" s="18"/>
       <c r="D52" s="18"/>
@@ -30676,10 +30678,10 @@
     </row>
     <row r="53" spans="1:5" ht="12.5">
       <c r="A53" s="18" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C53" s="18"/>
       <c r="D53" s="18"/>
@@ -30687,10 +30689,10 @@
     </row>
     <row r="54" spans="1:5" ht="12.5">
       <c r="A54" s="18" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C54" s="18"/>
       <c r="D54" s="18"/>
@@ -30698,10 +30700,10 @@
     </row>
     <row r="55" spans="1:5" ht="12.5">
       <c r="A55" s="18" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C55" s="18"/>
       <c r="D55" s="18"/>
@@ -30709,10 +30711,10 @@
     </row>
     <row r="56" spans="1:5" ht="12.5">
       <c r="A56" s="18" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C56" s="18"/>
       <c r="D56" s="18"/>
@@ -30720,10 +30722,10 @@
     </row>
     <row r="57" spans="1:5" ht="12.5">
       <c r="A57" s="18" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C57" s="18"/>
       <c r="D57" s="18"/>
@@ -30731,10 +30733,10 @@
     </row>
     <row r="58" spans="1:5" ht="12.5">
       <c r="A58" s="18" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C58" s="18"/>
       <c r="D58" s="18"/>
@@ -30742,10 +30744,10 @@
     </row>
     <row r="59" spans="1:5" ht="12.5">
       <c r="A59" s="18" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C59" s="18"/>
       <c r="D59" s="18"/>
@@ -30753,10 +30755,10 @@
     </row>
     <row r="60" spans="1:5" ht="12.5">
       <c r="A60" s="18" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C60" s="18"/>
       <c r="D60" s="18"/>
@@ -30764,10 +30766,10 @@
     </row>
     <row r="61" spans="1:5" ht="12.5">
       <c r="A61" s="18" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C61" s="18"/>
       <c r="D61" s="18"/>
@@ -30775,10 +30777,10 @@
     </row>
     <row r="62" spans="1:5" ht="12.5">
       <c r="A62" s="18" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C62" s="18"/>
       <c r="D62" s="18"/>
@@ -30786,10 +30788,10 @@
     </row>
     <row r="63" spans="1:5" ht="12.5">
       <c r="A63" s="18" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B63" s="18" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C63" s="18"/>
       <c r="D63" s="18"/>
@@ -30797,10 +30799,10 @@
     </row>
     <row r="64" spans="1:5" ht="12.5">
       <c r="A64" s="18" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C64" s="18"/>
       <c r="D64" s="18"/>
@@ -30808,10 +30810,10 @@
     </row>
     <row r="65" spans="1:5" ht="12.5">
       <c r="A65" s="18" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C65" s="18"/>
       <c r="D65" s="18"/>
@@ -30819,10 +30821,10 @@
     </row>
     <row r="66" spans="1:5" ht="12.5">
       <c r="A66" s="18" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C66" s="18"/>
       <c r="D66" s="18"/>
@@ -30830,10 +30832,10 @@
     </row>
     <row r="67" spans="1:5" ht="12.5">
       <c r="A67" s="18" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C67" s="18"/>
       <c r="D67" s="18"/>
@@ -30841,10 +30843,10 @@
     </row>
     <row r="68" spans="1:5" ht="12.5">
       <c r="A68" s="18" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C68" s="18"/>
       <c r="D68" s="18"/>
@@ -30852,10 +30854,10 @@
     </row>
     <row r="69" spans="1:5" ht="12.5">
       <c r="A69" s="18" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C69" s="18"/>
       <c r="D69" s="18"/>
@@ -30863,10 +30865,10 @@
     </row>
     <row r="70" spans="1:5" ht="12.5">
       <c r="A70" s="18" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C70" s="18"/>
       <c r="D70" s="18"/>
@@ -30874,10 +30876,10 @@
     </row>
     <row r="71" spans="1:5" ht="12.5">
       <c r="A71" s="18" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C71" s="18"/>
       <c r="D71" s="18"/>
@@ -30885,10 +30887,10 @@
     </row>
     <row r="72" spans="1:5" ht="12.5">
       <c r="A72" s="18" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C72" s="18"/>
       <c r="D72" s="18"/>
@@ -30896,10 +30898,10 @@
     </row>
     <row r="73" spans="1:5" ht="12.5">
       <c r="A73" s="18" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C73" s="18"/>
       <c r="D73" s="18"/>
@@ -30907,10 +30909,10 @@
     </row>
     <row r="74" spans="1:5" ht="12.5">
       <c r="A74" s="18" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C74" s="18"/>
       <c r="D74" s="18"/>
@@ -30918,10 +30920,10 @@
     </row>
     <row r="75" spans="1:5" ht="12.5">
       <c r="A75" s="18" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>285</v>
+        <v>369</v>
       </c>
       <c r="C75" s="18"/>
       <c r="D75" s="18"/>
@@ -30929,10 +30931,10 @@
     </row>
     <row r="76" spans="1:5" ht="12.5">
       <c r="A76" s="18" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C76" s="18"/>
       <c r="D76" s="18"/>
@@ -30941,7 +30943,7 @@
     <row r="77" spans="1:5" ht="12.5">
       <c r="A77" s="18"/>
       <c r="B77" s="18" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C77" s="18"/>
       <c r="D77" s="18"/>
@@ -30950,7 +30952,7 @@
     <row r="78" spans="1:5" ht="12.5">
       <c r="A78" s="18"/>
       <c r="B78" s="18" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C78" s="18"/>
       <c r="D78" s="18"/>
@@ -30959,7 +30961,7 @@
     <row r="79" spans="1:5" ht="12.5">
       <c r="A79" s="18"/>
       <c r="B79" s="18" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C79" s="18"/>
       <c r="D79" s="18"/>
@@ -30968,7 +30970,7 @@
     <row r="80" spans="1:5" ht="12.5">
       <c r="A80" s="18"/>
       <c r="B80" s="18" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C80" s="18"/>
       <c r="D80" s="18"/>
@@ -30977,7 +30979,7 @@
     <row r="81" spans="1:5" ht="12.5">
       <c r="A81" s="18"/>
       <c r="B81" s="18" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C81" s="18"/>
       <c r="D81" s="18"/>
@@ -30986,7 +30988,7 @@
     <row r="82" spans="1:5" ht="12.5">
       <c r="A82" s="18"/>
       <c r="B82" s="18" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C82" s="18"/>
       <c r="D82" s="18"/>
@@ -30995,7 +30997,7 @@
     <row r="83" spans="1:5" ht="12.5">
       <c r="A83" s="18"/>
       <c r="B83" s="18" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C83" s="18"/>
       <c r="D83" s="18"/>
@@ -31004,7 +31006,7 @@
     <row r="84" spans="1:5" ht="12.5">
       <c r="A84" s="18"/>
       <c r="B84" s="18" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C84" s="18"/>
       <c r="D84" s="18"/>
@@ -31013,7 +31015,7 @@
     <row r="85" spans="1:5" ht="12.5">
       <c r="A85" s="18"/>
       <c r="B85" s="18" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C85" s="18"/>
       <c r="D85" s="18"/>
@@ -31022,7 +31024,7 @@
     <row r="86" spans="1:5" ht="12.5">
       <c r="A86" s="18"/>
       <c r="B86" s="18" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C86" s="18"/>
       <c r="D86" s="18"/>
@@ -31031,7 +31033,7 @@
     <row r="87" spans="1:5" ht="12.5">
       <c r="A87" s="18"/>
       <c r="B87" s="18" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C87" s="18"/>
       <c r="D87" s="18"/>
@@ -31040,7 +31042,7 @@
     <row r="88" spans="1:5" ht="12.5">
       <c r="A88" s="18"/>
       <c r="B88" s="18" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C88" s="18"/>
       <c r="D88" s="18"/>
@@ -31049,7 +31051,7 @@
     <row r="89" spans="1:5" ht="12.5">
       <c r="A89" s="18"/>
       <c r="B89" s="18" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C89" s="18"/>
       <c r="D89" s="18"/>
@@ -31058,7 +31060,7 @@
     <row r="90" spans="1:5" ht="12.5">
       <c r="A90" s="18"/>
       <c r="B90" s="18" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C90" s="18"/>
       <c r="D90" s="18"/>
@@ -31079,8 +31081,8 @@
   </sheetPr>
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -31088,16 +31090,16 @@
     <col min="1" max="1" width="28.90625" customWidth="1"/>
     <col min="2" max="2" width="33.6328125" customWidth="1"/>
     <col min="3" max="3" width="30.26953125" customWidth="1"/>
-    <col min="4" max="4" width="45" customWidth="1"/>
+    <col min="4" max="4" width="19.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="35.5" customHeight="1">
-      <c r="A1" s="27" t="s">
-        <v>302</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="26"/>
+    <row r="1" spans="1:4" ht="15" customHeight="1">
+      <c r="A1" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1">
       <c r="A2" s="17" t="s">
@@ -31110,108 +31112,108 @@
         <v>128</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1">
       <c r="A3" s="18" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1">
       <c r="A4" s="18" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="23" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1">
       <c r="A5" s="18" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="23" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1">
       <c r="A6" s="18" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="23" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1">
       <c r="A7" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="23" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1">
       <c r="A8" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>61</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="23" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1">
       <c r="A9" s="18" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="23" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1">
       <c r="A10" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1">
       <c r="A11" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>132</v>
@@ -31221,7 +31223,7 @@
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1">
       <c r="A12" s="18" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>137</v>
@@ -31231,227 +31233,227 @@
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1">
       <c r="A13" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1">
       <c r="A14" s="18" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1">
       <c r="A15" s="18" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1">
       <c r="A16" s="18" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1">
       <c r="A17" s="18" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1">
       <c r="A18" s="18" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1">
       <c r="A19" s="18" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1">
       <c r="A20" s="18" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1">
       <c r="A21" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1">
       <c r="A22" s="18" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1">
       <c r="A23" s="18" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1">
       <c r="A24" s="18" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1">
       <c r="A25" s="18" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
     </row>
     <row r="26" spans="1:4" ht="12.5">
       <c r="A26" s="18" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
     </row>
     <row r="27" spans="1:4" ht="12.5">
       <c r="A27" s="18" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
     </row>
     <row r="28" spans="1:4" ht="12.5">
       <c r="A28" s="18" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
     </row>
     <row r="29" spans="1:4" ht="12.5">
       <c r="A29" s="18" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
     </row>
     <row r="30" spans="1:4" ht="12.5">
       <c r="A30" s="18" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="18"/>
     </row>
     <row r="31" spans="1:4" ht="12.5">
       <c r="A31" s="18" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C31" s="18"/>
       <c r="D31" s="18"/>
     </row>
     <row r="32" spans="1:4" ht="12.5">
       <c r="A32" s="18" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="18"/>
     </row>
     <row r="33" spans="1:4" ht="12.5">
       <c r="A33" s="18" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
     </row>
     <row r="34" spans="1:4" ht="12.5">
       <c r="A34" s="18" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
     </row>
     <row r="35" spans="1:4" ht="12.5">
       <c r="A35" s="18" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
@@ -31459,7 +31461,7 @@
     </row>
     <row r="36" spans="1:4" ht="12.5">
       <c r="A36" s="18" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
@@ -31467,7 +31469,7 @@
     </row>
     <row r="37" spans="1:4" ht="12.5">
       <c r="A37" s="18" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
@@ -31475,7 +31477,7 @@
     </row>
     <row r="38" spans="1:4" ht="12.5">
       <c r="A38" s="18" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B38" s="18"/>
       <c r="C38" s="18"/>
@@ -31483,7 +31485,7 @@
     </row>
     <row r="39" spans="1:4" ht="12.5">
       <c r="A39" s="18" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
@@ -31491,7 +31493,7 @@
     </row>
     <row r="40" spans="1:4" ht="12.5">
       <c r="A40" s="18" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B40" s="18"/>
       <c r="C40" s="18"/>
@@ -31499,7 +31501,7 @@
     </row>
     <row r="41" spans="1:4" ht="12.5">
       <c r="A41" s="18" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B41" s="18"/>
       <c r="C41" s="18"/>
@@ -31507,7 +31509,7 @@
     </row>
     <row r="42" spans="1:4" ht="12.5">
       <c r="A42" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B42" s="18"/>
       <c r="C42" s="18"/>
@@ -31515,7 +31517,7 @@
     </row>
     <row r="43" spans="1:4" ht="12.5">
       <c r="A43" s="18" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B43" s="18"/>
       <c r="C43" s="18"/>
@@ -31523,7 +31525,7 @@
     </row>
     <row r="44" spans="1:4" ht="12.5">
       <c r="A44" s="18" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B44" s="18"/>
       <c r="C44" s="18"/>
@@ -31531,7 +31533,7 @@
     </row>
     <row r="45" spans="1:4" ht="12.5">
       <c r="A45" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B45" s="18"/>
       <c r="C45" s="18"/>
@@ -31539,7 +31541,7 @@
     </row>
     <row r="46" spans="1:4" ht="12.5">
       <c r="A46" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B46" s="18"/>
       <c r="C46" s="18"/>
@@ -31547,7 +31549,7 @@
     </row>
     <row r="47" spans="1:4" ht="12.5">
       <c r="A47" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B47" s="18"/>
       <c r="C47" s="18"/>
@@ -31555,7 +31557,7 @@
     </row>
     <row r="48" spans="1:4" ht="12.5">
       <c r="A48" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B48" s="18"/>
       <c r="C48" s="18"/>
@@ -31563,7 +31565,7 @@
     </row>
     <row r="49" spans="1:4" ht="12.5">
       <c r="A49" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B49" s="18"/>
       <c r="C49" s="18"/>
@@ -31571,7 +31573,7 @@
     </row>
     <row r="50" spans="1:4" ht="12.5">
       <c r="A50" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B50" s="18"/>
       <c r="C50" s="18"/>
@@ -31579,7 +31581,7 @@
     </row>
     <row r="51" spans="1:4" ht="12.5">
       <c r="A51" s="18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B51" s="18"/>
       <c r="C51" s="18"/>
@@ -31587,7 +31589,7 @@
     </row>
     <row r="52" spans="1:4" ht="12.5">
       <c r="A52" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B52" s="18"/>
       <c r="C52" s="18"/>
@@ -31595,7 +31597,7 @@
     </row>
     <row r="53" spans="1:4" ht="12.5">
       <c r="A53" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B53" s="18"/>
       <c r="C53" s="18"/>
@@ -31603,7 +31605,7 @@
     </row>
     <row r="54" spans="1:4" ht="12.5">
       <c r="A54" s="18" t="s">
-        <v>218</v>
+        <v>367</v>
       </c>
       <c r="B54" s="18"/>
       <c r="C54" s="18"/>
@@ -31611,7 +31613,7 @@
     </row>
     <row r="55" spans="1:4" ht="12.5">
       <c r="A55" s="18" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B55" s="18"/>
       <c r="C55" s="18"/>
@@ -31619,7 +31621,7 @@
     </row>
     <row r="56" spans="1:4" ht="12.5">
       <c r="A56" s="18" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B56" s="18"/>
       <c r="C56" s="18"/>
@@ -31627,7 +31629,7 @@
     </row>
     <row r="57" spans="1:4" ht="12.5">
       <c r="A57" s="18" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B57" s="18"/>
       <c r="C57" s="18"/>
@@ -31635,7 +31637,7 @@
     </row>
     <row r="58" spans="1:4" ht="12.5">
       <c r="A58" s="18" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B58" s="18"/>
       <c r="C58" s="18"/>
@@ -31643,7 +31645,7 @@
     </row>
     <row r="59" spans="1:4" ht="12.5">
       <c r="A59" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B59" s="18"/>
       <c r="C59" s="18"/>
@@ -31651,7 +31653,7 @@
     </row>
     <row r="60" spans="1:4" ht="12.5">
       <c r="A60" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B60" s="18"/>
       <c r="C60" s="18"/>
@@ -31659,7 +31661,7 @@
     </row>
     <row r="61" spans="1:4" ht="12.5">
       <c r="A61" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B61" s="18"/>
       <c r="C61" s="18"/>
@@ -31667,7 +31669,7 @@
     </row>
     <row r="62" spans="1:4" ht="12.5">
       <c r="A62" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B62" s="18"/>
       <c r="C62" s="18"/>
@@ -31675,7 +31677,7 @@
     </row>
     <row r="63" spans="1:4" ht="12.5">
       <c r="A63" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B63" s="18"/>
       <c r="C63" s="18"/>
@@ -31683,7 +31685,7 @@
     </row>
     <row r="64" spans="1:4" ht="12.5">
       <c r="A64" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B64" s="18"/>
       <c r="C64" s="18"/>
@@ -31691,7 +31693,7 @@
     </row>
     <row r="65" spans="1:4" ht="12.5">
       <c r="A65" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B65" s="18"/>
       <c r="C65" s="18"/>
@@ -31699,7 +31701,7 @@
     </row>
     <row r="66" spans="1:4" ht="12.5">
       <c r="A66" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B66" s="18"/>
       <c r="C66" s="18"/>
@@ -31707,7 +31709,7 @@
     </row>
     <row r="67" spans="1:4" ht="12.5">
       <c r="A67" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B67" s="18"/>
       <c r="C67" s="18"/>
@@ -31715,7 +31717,7 @@
     </row>
     <row r="68" spans="1:4" ht="12.5">
       <c r="A68" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B68" s="18"/>
       <c r="C68" s="18"/>
@@ -31723,7 +31725,7 @@
     </row>
     <row r="69" spans="1:4" ht="12.5">
       <c r="A69" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B69" s="18"/>
       <c r="C69" s="18"/>
@@ -31731,7 +31733,7 @@
     </row>
     <row r="70" spans="1:4" ht="12.5">
       <c r="A70" s="18" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B70" s="18"/>
       <c r="C70" s="18"/>
@@ -31739,7 +31741,7 @@
     </row>
     <row r="71" spans="1:4" ht="12.5">
       <c r="A71" s="18" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B71" s="18"/>
       <c r="C71" s="18"/>
@@ -31747,7 +31749,7 @@
     </row>
     <row r="72" spans="1:4" ht="12.5">
       <c r="A72" s="18" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B72" s="18"/>
       <c r="C72" s="18"/>
@@ -31755,7 +31757,7 @@
     </row>
     <row r="73" spans="1:4" ht="12.5">
       <c r="A73" s="18" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B73" s="18"/>
       <c r="C73" s="18"/>
@@ -31763,7 +31765,7 @@
     </row>
     <row r="74" spans="1:4" ht="12.5">
       <c r="A74" s="18" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B74" s="18"/>
       <c r="C74" s="18"/>
@@ -31771,7 +31773,7 @@
     </row>
     <row r="75" spans="1:4" ht="12.5">
       <c r="A75" s="18" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B75" s="18"/>
       <c r="C75" s="18"/>
@@ -31779,7 +31781,7 @@
     </row>
     <row r="76" spans="1:4" ht="12.5">
       <c r="A76" s="18" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B76" s="18"/>
       <c r="C76" s="18"/>
@@ -31787,7 +31789,7 @@
     </row>
     <row r="77" spans="1:4" ht="12.5">
       <c r="A77" s="18" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B77" s="18"/>
       <c r="C77" s="18"/>
@@ -31795,7 +31797,7 @@
     </row>
     <row r="78" spans="1:4" ht="12.5">
       <c r="A78" s="18" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B78" s="18"/>
       <c r="C78" s="18"/>
@@ -31803,7 +31805,7 @@
     </row>
     <row r="79" spans="1:4" ht="12.5">
       <c r="A79" s="18" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B79" s="18"/>
       <c r="C79" s="18"/>
@@ -31811,7 +31813,7 @@
     </row>
     <row r="80" spans="1:4" ht="12.5">
       <c r="A80" s="18" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B80" s="18"/>
       <c r="C80" s="18"/>
@@ -31819,7 +31821,7 @@
     </row>
     <row r="81" spans="1:4" ht="12.5">
       <c r="A81" s="18" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B81" s="18"/>
       <c r="C81" s="18"/>
@@ -31827,7 +31829,7 @@
     </row>
     <row r="82" spans="1:4" ht="12.5">
       <c r="A82" s="18" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B82" s="18"/>
       <c r="C82" s="18"/>
@@ -31835,7 +31837,7 @@
     </row>
     <row r="83" spans="1:4" ht="12.5">
       <c r="A83" s="18" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B83" s="18"/>
       <c r="C83" s="18"/>
@@ -31843,7 +31845,7 @@
     </row>
     <row r="84" spans="1:4" ht="12.5">
       <c r="A84" s="18" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B84" s="18"/>
       <c r="C84" s="18"/>
@@ -31851,7 +31853,7 @@
     </row>
     <row r="85" spans="1:4" ht="12.5">
       <c r="A85" s="18" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B85" s="18"/>
       <c r="C85" s="18"/>
@@ -31859,7 +31861,7 @@
     </row>
     <row r="86" spans="1:4" ht="12.5">
       <c r="A86" s="18" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B86" s="18"/>
       <c r="C86" s="18"/>
@@ -31867,7 +31869,7 @@
     </row>
     <row r="87" spans="1:4" ht="12.5">
       <c r="A87" s="18" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B87" s="18"/>
       <c r="C87" s="18"/>
@@ -31875,7 +31877,7 @@
     </row>
     <row r="88" spans="1:4" ht="12.5">
       <c r="A88" s="18" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B88" s="18"/>
       <c r="C88" s="18"/>
@@ -31883,7 +31885,7 @@
     </row>
     <row r="89" spans="1:4" ht="12.5">
       <c r="A89" s="18" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B89" s="18"/>
       <c r="C89" s="18"/>
@@ -31891,7 +31893,7 @@
     </row>
     <row r="90" spans="1:4" ht="12.5">
       <c r="A90" s="18" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B90" s="18"/>
       <c r="C90" s="18"/>
@@ -31899,7 +31901,7 @@
     </row>
     <row r="91" spans="1:4" ht="12.5">
       <c r="A91" s="18" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B91" s="18"/>
       <c r="C91" s="18"/>
@@ -31907,7 +31909,7 @@
     </row>
     <row r="92" spans="1:4" ht="12.5">
       <c r="A92" s="18" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B92" s="18"/>
       <c r="C92" s="18"/>
@@ -31934,7 +31936,9 @@
   </sheetPr>
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -31943,72 +31947,72 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1">
       <c r="A1" s="17" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15" customHeight="1">
       <c r="A2" s="24" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15" customHeight="1">
       <c r="A3" s="24" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15" customHeight="1">
       <c r="A4" s="24" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15" customHeight="1">
       <c r="A5" s="24" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15" customHeight="1">
       <c r="A6" s="24" t="s">
-        <v>77</v>
+        <v>366</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15" customHeight="1">
       <c r="A7" s="24" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15" customHeight="1">
       <c r="A8" s="24" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15" customHeight="1">
       <c r="A9" s="24" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15" customHeight="1">
       <c r="A10" s="24" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15" customHeight="1">
       <c r="A11" s="24" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15" customHeight="1">
       <c r="A12" s="24" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15" customHeight="1">
       <c r="A13" s="24" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15" customHeight="1">
       <c r="A14" s="24" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Report, Excel and tar update
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/IngredientsAndComorbidities-ScrapperHackathon.xlsx
+++ b/src/test/resources/testdata/IngredientsAndComorbidities-ScrapperHackathon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Febi\NumpyNinja\Hackathon\RecipeScrapingHackathon_July24\RecipeScraping\Team11_ScrapeTechies_ScrapingHackthonJuly24\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49D9FCA-AB4C-4EF7-92CA-C3044E74BD19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8F7AC1-345F-4033-9290-7EEDE0CB1CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="374">
   <si>
     <t>Diabetes</t>
   </si>
@@ -1141,6 +1141,15 @@
   </si>
   <si>
     <t>microwave</t>
+  </si>
+  <si>
+    <t>corn flakes</t>
+  </si>
+  <si>
+    <t>icecream</t>
+  </si>
+  <si>
+    <t>ice-cream</t>
   </si>
 </sst>
 </file>
@@ -1721,7 +1730,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -30057,7 +30066,7 @@
   <dimension ref="A1:J90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -30072,7 +30081,7 @@
     <col min="10" max="10" width="18.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1">
+    <row r="1" spans="1:8" ht="31" customHeight="1">
       <c r="A1" s="28" t="s">
         <v>125</v>
       </c>
@@ -30941,7 +30950,9 @@
       <c r="E76" s="18"/>
     </row>
     <row r="77" spans="1:5" ht="12.5">
-      <c r="A77" s="18"/>
+      <c r="A77" s="18" t="s">
+        <v>371</v>
+      </c>
       <c r="B77" s="18" t="s">
         <v>284</v>
       </c>
@@ -30950,7 +30961,9 @@
       <c r="E77" s="18"/>
     </row>
     <row r="78" spans="1:5" ht="12.5">
-      <c r="A78" s="18"/>
+      <c r="A78" s="18" t="s">
+        <v>373</v>
+      </c>
       <c r="B78" s="18" t="s">
         <v>285</v>
       </c>
@@ -30959,7 +30972,9 @@
       <c r="E78" s="18"/>
     </row>
     <row r="79" spans="1:5" ht="12.5">
-      <c r="A79" s="18"/>
+      <c r="A79" s="18" t="s">
+        <v>372</v>
+      </c>
       <c r="B79" s="18" t="s">
         <v>286</v>
       </c>
@@ -31079,9 +31094,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
+    <sheetView topLeftCell="A79" workbookViewId="0">
       <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
@@ -31916,10 +31931,17 @@
       <c r="D92" s="18"/>
     </row>
     <row r="93" spans="1:4" ht="12.5">
-      <c r="A93" s="18"/>
+      <c r="A93" s="18" t="s">
+        <v>373</v>
+      </c>
       <c r="B93" s="18"/>
       <c r="C93" s="18"/>
       <c r="D93" s="18"/>
+    </row>
+    <row r="94" spans="1:4" ht="15" customHeight="1">
+      <c r="A94" s="18" t="s">
+        <v>372</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -31937,7 +31959,7 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>